<commit_message>
updates in gui for real_time Checks.
</commit_message>
<xml_diff>
--- a/Data/ticket_data.xlsx
+++ b/Data/ticket_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,46 +458,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bheru</t>
+          <t>ayush</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>bheru@paytm</t>
+          <t>aj@pytm</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>c62bbd77005c0abc</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>ea731e88696ba970</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>shubham</t>
+          <t>bheru</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>shubham@paypal</t>
+          <t>bheru@paypal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>bb0d2115b586a1c5</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>8c6d0751770bfc06</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -507,47 +499,127 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dinesh@razorpay</t>
+          <t>din@gpay</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>a6fe557d618c222f</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>aa424ef629984b38</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>shubham</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>shubh@gpay</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>c6e8fcbd208e2924</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ayush</t>
+          <t>satyen</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ayush@paytm</t>
+          <t>asat@razorpay</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>333d1cd23619697a</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+          <t>6f80e78819a17332</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>a@payed</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>da9026abc665025c</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>b@payed</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>cfaea30e3b402902</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>c@payed</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4d795f2d3f2296c2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>d4</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>d@payed</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>7cd82693b24af5f3</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>